<commit_message>
Fixed bugs caused by restructuring for git
</commit_message>
<xml_diff>
--- a/Analyses/_templateAnalysis/config.xlsx
+++ b/Analyses/_templateAnalysis/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Michiel/Dimple - Working Documents/DimpleTech/10 Technology development/01 The Hill/03 Usage/Analyses/_templateAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AD23A1-2DE6-9743-A92E-4D0E49393727}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{825C4B77-2322-164C-AB22-7D4235288779}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="17060" windowHeight="14000" xr2:uid="{56C23509-9F59-254D-8F85-61859C64460F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="26780" xr2:uid="{56C23509-9F59-254D-8F85-61859C64460F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>ID 1</t>
   </si>
@@ -173,12 +173,81 @@
   <si>
     <t>marker (opt)</t>
   </si>
+  <si>
+    <t>Line</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Marker</t>
+  </si>
+  <si>
+    <t>color (opt)</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t>^</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>-.</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -199,6 +268,12 @@
       <sz val="12"/>
       <color theme="1" tint="0.499984740745262"/>
       <name val="Calibri (Body)_x0000_"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFA020F0"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -254,13 +329,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,7 +652,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F400611F-347A-1F48-877C-560D573914B1}">
-  <dimension ref="B2:G15"/>
+  <dimension ref="B2:L15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
@@ -584,9 +661,10 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="9" max="11" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7">
+    <row r="2" spans="2:12">
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
@@ -594,7 +672,7 @@
         <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>14</v>
@@ -602,22 +680,46 @@
       <c r="G2" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="2:7">
+      <c r="I2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12">
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="2:7">
+      <c r="E3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -626,8 +728,18 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="2:7">
+      <c r="I4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="6"/>
+    </row>
+    <row r="5" spans="2:12">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -636,8 +748,17 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="2:7">
+      <c r="I5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -646,8 +767,17 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="2:7">
+      <c r="I6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -656,8 +786,14 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="2:7">
+      <c r="I7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -666,8 +802,14 @@
       <c r="E8" s="3"/>
       <c r="F8" s="5"/>
       <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="2:7">
+      <c r="I8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -676,8 +818,11 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="2:7">
+      <c r="K9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -686,8 +831,11 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="2:7">
+      <c r="K10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12">
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -696,8 +844,11 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="2:7">
+      <c r="K11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -707,20 +858,29 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="14" spans="2:7" hidden="1">
+    <row r="14" spans="2:12" hidden="1">
       <c r="D14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:7" hidden="1">
+    <row r="15" spans="2:12" hidden="1">
       <c r="D15" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D12" xr:uid="{B911E480-FF24-DD49-AE4B-700898E35F11}">
       <formula1>$D$14:$D$15</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E12" xr:uid="{2913578C-40CD-C245-82C6-20C4327C6B46}">
+      <formula1>$I$3:$I$8</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F12" xr:uid="{998D9A91-7C02-DB46-96E5-1C49848ACE11}">
+      <formula1>$J$3:$J$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G12" xr:uid="{6EAB8B87-5C0E-D947-9120-AD2D3E0515E0}">
+      <formula1>$K$3:$K$11</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Custom measurements names and pressure data bug
</commit_message>
<xml_diff>
--- a/Analyses/_templateAnalysis/config.xlsx
+++ b/Analyses/_templateAnalysis/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Michiel/Dimple - Working Documents/DimpleTech/10 Technology development/01 The Hill/03 Usage/Analyses/_templateAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{825C4B77-2322-164C-AB22-7D4235288779}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813C1BAE-FB66-6749-A7B5-1E56F50E5B9C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="26780" xr2:uid="{56C23509-9F59-254D-8F85-61859C64460F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13860" xr2:uid="{56C23509-9F59-254D-8F85-61859C64460F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>ID 1</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>c</t>
+  </si>
+  <si>
+    <t>Custom name</t>
   </si>
 </sst>
 </file>
@@ -655,13 +658,16 @@
   <dimension ref="B2:L15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="9" max="11" width="0" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="26.33203125" customWidth="1"/>
+    <col min="9" max="10" width="0" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12">
@@ -680,6 +686,9 @@
       <c r="G2" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H2" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="I2" s="2" t="s">
         <v>17</v>
       </c>
@@ -697,18 +706,11 @@
       <c r="C3" s="1">
         <v>0</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
       <c r="I3" t="s">
         <v>33</v>
       </c>
@@ -728,6 +730,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
       <c r="I4" t="s">
         <v>34</v>
       </c>
@@ -748,6 +751,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
       <c r="I5" t="s">
         <v>35</v>
       </c>
@@ -767,6 +771,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
       <c r="I6" t="s">
         <v>36</v>
       </c>
@@ -786,6 +791,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
       <c r="I7" t="s">
         <v>37</v>
       </c>
@@ -802,6 +808,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="5"/>
       <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
       <c r="I8" t="s">
         <v>38</v>
       </c>
@@ -818,6 +825,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
       <c r="K9" t="s">
         <v>26</v>
       </c>
@@ -831,6 +839,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
       <c r="K10" t="s">
         <v>27</v>
       </c>
@@ -844,6 +853,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
       <c r="K11" t="s">
         <v>28</v>
       </c>
@@ -857,6 +867,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
     </row>
     <row r="14" spans="2:12" hidden="1">
       <c r="D14" t="s">

</xml_diff>

<commit_message>
Update saveAllFigures and gitignore
</commit_message>
<xml_diff>
--- a/Analyses/_templateAnalysis/config.xlsx
+++ b/Analyses/_templateAnalysis/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Michiel/Dimple - Working Documents/DimpleTech/10 Technology development/01 The Hill/03 Usage/Analyses/_templateAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813C1BAE-FB66-6749-A7B5-1E56F50E5B9C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C219611-FC04-C549-A793-2B41FCBB8A47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13860" xr2:uid="{56C23509-9F59-254D-8F85-61859C64460F}"/>
   </bookViews>
@@ -658,7 +658,7 @@
   <dimension ref="B2:L15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -704,7 +704,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>0</v>
+        <v>281</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="3"/>

</xml_diff>

<commit_message>
Update template analysis config
</commit_message>
<xml_diff>
--- a/Analyses/_templateAnalysis/config.xlsx
+++ b/Analyses/_templateAnalysis/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Michiel/Dimple - Working Documents/DimpleTech/10 Technology development/01 The Hill/03 Usage/Analyses/_templateAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C219611-FC04-C549-A793-2B41FCBB8A47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61C56F14-A2EC-AD4D-81BD-D5D412F42DE6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13860" xr2:uid="{56C23509-9F59-254D-8F85-61859C64460F}"/>
   </bookViews>
@@ -704,7 +704,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>281</v>
+        <v>0</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="3"/>

</xml_diff>